<commit_message>
Update extension QR 46e15d5e7e8798dcee299f94163276ff9e819b94
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-26T11:13:08+00:00</t>
+    <t>2025-09-26T13:47:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -450,17 +450,17 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>QuestionnaireResponse.extension:TDDUIAuthor</t>
-  </si>
-  <si>
-    <t>TDDUIAuthor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-auhtor}
+    <t>QuestionnaireResponse.extension:TDDUIResponsible</t>
+  </si>
+  <si>
+    <t>TDDUIResponsible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-responsible}
 </t>
   </si>
   <si>
-    <t>Auteur de l'évaluation</t>
+    <t>Responsable de l'évaluation</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1

</xml_diff>

<commit_message>
Ajout exemples évaluation e853bea5e137a0d200fb8bf9ef9802b60df82554
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-29T08:20:50+00:00</t>
+    <t>2025-09-29T14:52:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -590,7 +590,11 @@
 </t>
   </si>
   <si>
-    <t>Form being answered</t>
+    <t>Le profil permet de communiquer les grilles définies suivantes :
+- Evaluation AGGIR PA SSIAD
+- Evaluation AGGIR PH SSIAD
+- Evaluation SERAFIN
+- Evaluation situation SSIAD</t>
   </si>
   <si>
     <t>The Questionnaire that defines and organizes the questions for which answers are being provided.</t>

</xml_diff>

<commit_message>
Remove item commentaire e4080ded9b4b936e05ae55a44638d89fb9101f93
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-questionnaire-response.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="445">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-06T14:50:01+00:00</t>
+    <t>2025-10-07T08:55:00+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1349,12 +1349,6 @@
   </si>
   <si>
     <t>QuestionnaireResponse.item.item.answer.value[x]</t>
-  </si>
-  <si>
-    <t>QuestionnaireResponse.item.item.answer.value[x]:valueString</t>
-  </si>
-  <si>
-    <t>valueString</t>
   </si>
   <si>
     <t>QuestionnaireResponse.item.item.answer.item</t>
@@ -1710,7 +1704,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO90"/>
+  <dimension ref="A1:AO89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -10262,14 +10256,16 @@
         <v>81</v>
       </c>
       <c r="AB73" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="AC73" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="AD73" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>395</v>
@@ -10307,11 +10303,9 @@
         <v>428</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="C74" t="s" s="2">
-        <v>429</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
         <v>81</v>
       </c>
@@ -10320,7 +10314,7 @@
         <v>79</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>81</v>
@@ -10332,19 +10326,17 @@
         <v>81</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>81</v>
@@ -10369,13 +10361,13 @@
         <v>81</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>401</v>
+        <v>81</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>402</v>
+        <v>81</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>81</v>
@@ -10393,13 +10385,13 @@
         <v>81</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH74" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AI74" t="s" s="2">
         <v>81</v>
@@ -10408,7 +10400,7 @@
         <v>104</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>363</v>
+        <v>81</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>81</v>
@@ -10417,7 +10409,7 @@
         <v>81</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>404</v>
+        <v>359</v>
       </c>
       <c r="AO74" t="s" s="2">
         <v>81</v>
@@ -10425,10 +10417,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10451,17 +10443,17 @@
         <v>81</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>82</v>
+        <v>353</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="P75" t="s" s="2">
         <v>81</v>
@@ -10510,7 +10502,7 @@
         <v>81</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -10525,7 +10517,7 @@
         <v>104</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>81</v>
+        <v>430</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>81</v>
@@ -10556,7 +10548,7 @@
         <v>79</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>81</v>
@@ -10568,18 +10560,16 @@
         <v>81</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>353</v>
+        <v>106</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>413</v>
+        <v>107</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>414</v>
+        <v>108</v>
       </c>
       <c r="N76" s="2"/>
-      <c r="O76" t="s" s="2">
-        <v>415</v>
-      </c>
+      <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
         <v>81</v>
       </c>
@@ -10627,22 +10617,22 @@
         <v>81</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>412</v>
+        <v>109</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH76" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>432</v>
+        <v>81</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>81</v>
@@ -10651,7 +10641,7 @@
         <v>81</v>
       </c>
       <c r="AN76" t="s" s="2">
-        <v>359</v>
+        <v>110</v>
       </c>
       <c r="AO76" t="s" s="2">
         <v>81</v>
@@ -10659,10 +10649,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10673,7 +10663,7 @@
         <v>79</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>81</v>
@@ -10685,13 +10675,13 @@
         <v>81</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>108</v>
+        <v>195</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -10730,31 +10720,29 @@
         <v>81</v>
       </c>
       <c r="AB77" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>81</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="AC77" s="2"/>
       <c r="AD77" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>81</v>
@@ -10766,7 +10754,7 @@
         <v>81</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="AO77" t="s" s="2">
         <v>81</v>
@@ -10774,12 +10762,14 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>434</v>
-      </c>
-      <c r="C78" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="C78" t="s" s="2">
+        <v>246</v>
+      </c>
       <c r="D78" t="s" s="2">
         <v>81</v>
       </c>
@@ -10788,7 +10778,7 @@
         <v>79</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>81</v>
@@ -10800,13 +10790,13 @@
         <v>81</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>194</v>
+        <v>248</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -10845,14 +10835,16 @@
         <v>81</v>
       </c>
       <c r="AB78" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="AC78" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="AC78" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="AD78" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>120</v>
@@ -10864,13 +10856,13 @@
         <v>80</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="AJ78" t="s" s="2">
         <v>121</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>81</v>
+        <v>363</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>81</v>
@@ -10887,44 +10879,46 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="C79" t="s" s="2">
-        <v>246</v>
-      </c>
+      <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
-        <v>81</v>
+        <v>365</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G79" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H79" t="s" s="2">
         <v>81</v>
       </c>
       <c r="I79" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>248</v>
+        <v>366</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
+        <v>367</v>
+      </c>
+      <c r="N79" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="O79" t="s" s="2">
+        <v>254</v>
+      </c>
       <c r="P79" t="s" s="2">
         <v>81</v>
       </c>
@@ -10972,7 +10966,7 @@
         <v>81</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>120</v>
+        <v>368</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>79</v>
@@ -10981,13 +10975,13 @@
         <v>80</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>202</v>
+        <v>81</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>121</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>363</v>
+        <v>81</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>81</v>
@@ -10996,7 +10990,7 @@
         <v>81</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>81</v>
+        <v>192</v>
       </c>
       <c r="AO79" t="s" s="2">
         <v>81</v>
@@ -11004,45 +10998,43 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
-        <v>365</v>
+        <v>81</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H80" t="s" s="2">
         <v>81</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>116</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
-        <v>254</v>
+        <v>372</v>
       </c>
       <c r="P80" t="s" s="2">
         <v>81</v>
@@ -11091,22 +11083,22 @@
         <v>81</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="AH80" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AI80" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>81</v>
+        <v>373</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>81</v>
@@ -11115,7 +11107,7 @@
         <v>81</v>
       </c>
       <c r="AN80" t="s" s="2">
-        <v>192</v>
+        <v>374</v>
       </c>
       <c r="AO80" t="s" s="2">
         <v>81</v>
@@ -11123,10 +11115,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11134,7 +11126,7 @@
       </c>
       <c r="E81" s="2"/>
       <c r="F81" t="s" s="2">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G81" t="s" s="2">
         <v>92</v>
@@ -11149,17 +11141,19 @@
         <v>81</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="N81" s="2"/>
+        <v>377</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>378</v>
+      </c>
       <c r="O81" t="s" s="2">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="P81" t="s" s="2">
         <v>81</v>
@@ -11208,10 +11202,10 @@
         <v>81</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="AH81" t="s" s="2">
         <v>92</v>
@@ -11223,7 +11217,7 @@
         <v>104</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>373</v>
+        <v>81</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>81</v>
@@ -11232,7 +11226,7 @@
         <v>81</v>
       </c>
       <c r="AN81" t="s" s="2">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="AO81" t="s" s="2">
         <v>81</v>
@@ -11240,10 +11234,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11266,19 +11260,17 @@
         <v>81</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="N82" t="s" s="2">
-        <v>378</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="P82" t="s" s="2">
         <v>81</v>
@@ -11327,7 +11319,7 @@
         <v>81</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>79</v>
@@ -11351,7 +11343,7 @@
         <v>81</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="AO82" t="s" s="2">
         <v>81</v>
@@ -11359,10 +11351,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11373,7 +11365,7 @@
         <v>79</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>81</v>
@@ -11385,18 +11377,18 @@
         <v>81</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>106</v>
+        <v>353</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="N83" s="2"/>
-      <c r="O83" t="s" s="2">
-        <v>384</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
         <v>81</v>
       </c>
@@ -11444,13 +11436,13 @@
         <v>81</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>81</v>
@@ -11459,7 +11451,7 @@
         <v>104</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>81</v>
+        <v>390</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>81</v>
@@ -11468,7 +11460,7 @@
         <v>81</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="AO83" t="s" s="2">
         <v>81</v>
@@ -11476,10 +11468,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -11490,7 +11482,7 @@
         <v>79</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H84" t="s" s="2">
         <v>81</v>
@@ -11502,17 +11494,15 @@
         <v>81</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>353</v>
+        <v>106</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>387</v>
+        <v>107</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>389</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
         <v>81</v>
@@ -11561,22 +11551,22 @@
         <v>81</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>386</v>
+        <v>109</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH84" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AI84" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>390</v>
+        <v>81</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>81</v>
@@ -11585,7 +11575,7 @@
         <v>81</v>
       </c>
       <c r="AN84" t="s" s="2">
-        <v>391</v>
+        <v>110</v>
       </c>
       <c r="AO84" t="s" s="2">
         <v>81</v>
@@ -11593,21 +11583,21 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H85" t="s" s="2">
         <v>81</v>
@@ -11619,15 +11609,17 @@
         <v>81</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N85" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>116</v>
+      </c>
       <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
         <v>81</v>
@@ -11676,19 +11668,19 @@
         <v>81</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>81</v>
@@ -11708,14 +11700,14 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
-        <v>112</v>
+        <v>365</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" t="s" s="2">
@@ -11728,24 +11720,26 @@
         <v>81</v>
       </c>
       <c r="I86" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="K86" t="s" s="2">
         <v>113</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>114</v>
+        <v>366</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>115</v>
+        <v>367</v>
       </c>
       <c r="N86" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="O86" s="2"/>
+      <c r="O86" t="s" s="2">
+        <v>254</v>
+      </c>
       <c r="P86" t="s" s="2">
         <v>81</v>
       </c>
@@ -11793,7 +11787,7 @@
         <v>81</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>120</v>
+        <v>368</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>79</v>
@@ -11817,7 +11811,7 @@
         <v>81</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>81</v>
@@ -11825,45 +11819,45 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>365</v>
+        <v>81</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>81</v>
       </c>
       <c r="I87" t="s" s="2">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>113</v>
+        <v>396</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>366</v>
+        <v>397</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>367</v>
+        <v>398</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>116</v>
+        <v>399</v>
       </c>
       <c r="O87" t="s" s="2">
-        <v>254</v>
+        <v>400</v>
       </c>
       <c r="P87" t="s" s="2">
         <v>81</v>
@@ -11888,13 +11882,13 @@
         <v>81</v>
       </c>
       <c r="X87" t="s" s="2">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="Y87" t="s" s="2">
-        <v>81</v>
+        <v>401</v>
       </c>
       <c r="Z87" t="s" s="2">
-        <v>81</v>
+        <v>402</v>
       </c>
       <c r="AA87" t="s" s="2">
         <v>81</v>
@@ -11912,19 +11906,19 @@
         <v>81</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH87" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AI87" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>81</v>
@@ -11936,7 +11930,7 @@
         <v>81</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>192</v>
+        <v>404</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>81</v>
@@ -11944,10 +11938,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -11958,7 +11952,7 @@
         <v>79</v>
       </c>
       <c r="G88" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H88" t="s" s="2">
         <v>81</v>
@@ -11970,19 +11964,17 @@
         <v>81</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>396</v>
+        <v>82</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="P88" t="s" s="2">
         <v>81</v>
@@ -12007,13 +11999,13 @@
         <v>81</v>
       </c>
       <c r="X88" t="s" s="2">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="Y88" t="s" s="2">
-        <v>401</v>
+        <v>81</v>
       </c>
       <c r="Z88" t="s" s="2">
-        <v>402</v>
+        <v>81</v>
       </c>
       <c r="AA88" t="s" s="2">
         <v>81</v>
@@ -12031,13 +12023,13 @@
         <v>81</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH88" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AI88" t="s" s="2">
         <v>81</v>
@@ -12055,7 +12047,7 @@
         <v>81</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>404</v>
+        <v>359</v>
       </c>
       <c r="AO88" t="s" s="2">
         <v>81</v>
@@ -12063,10 +12055,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12092,14 +12084,14 @@
         <v>82</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="P89" t="s" s="2">
         <v>81</v>
@@ -12148,7 +12140,7 @@
         <v>81</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -12175,123 +12167,6 @@
         <v>359</v>
       </c>
       <c r="AO89" t="s" s="2">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>446</v>
-      </c>
-      <c r="B90" t="s" s="2">
-        <v>446</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="E90" s="2"/>
-      <c r="F90" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="G90" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="H90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="I90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="J90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="K90" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="M90" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="N90" s="2"/>
-      <c r="O90" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="P90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Q90" s="2"/>
-      <c r="R90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="S90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="T90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="U90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="V90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="W90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="X90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Y90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Z90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AA90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AB90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AC90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AD90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AE90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AF90" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="AG90" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AH90" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AJ90" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AK90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AL90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AM90" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AN90" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="AO90" t="s" s="2">
         <v>81</v>
       </c>
     </row>

</xml_diff>